<commit_message>
fix model and tests
</commit_message>
<xml_diff>
--- a/model/tests/resources/letters.xlsx
+++ b/model/tests/resources/letters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>א</t>
   </si>
@@ -216,13 +216,19 @@
   </si>
   <si>
     <t>NONE</t>
+  </si>
+  <si>
+    <t>ֻ</t>
+  </si>
+  <si>
+    <t>ֻּ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +236,19 @@
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -252,11 +271,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -841,11 +864,17 @@
       <c r="A28" t="s">
         <v>27</v>
       </c>
+      <c r="B28" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>25</v>
       </c>
+      <c r="B29" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -874,5 +903,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>